<commit_message>
Meeting answer and gitignore update
</commit_message>
<xml_diff>
--- a/publi/checks.xlsx
+++ b/publi/checks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\melvy\Desktop\Dev\2022-herzig\publi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{326C726A-B95A-4412-BEC8-1EA9C88F8052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0E7150E-C0B6-4B42-95EA-D2CE0FCF9736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="915" windowWidth="26505" windowHeight="14100" xr2:uid="{7459B878-47C4-4386-AB9E-890DDB192382}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7459B878-47C4-4386-AB9E-890DDB192382}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -100,9 +100,6 @@
     <t xml:space="preserve">Request </t>
   </si>
   <si>
-    <t xml:space="preserve">Si des requêtes sont présentes les ignorer ? </t>
-  </si>
-  <si>
     <t>Vérifier que la valeur d'un sample ne soit pas en dessous du 0 pourcent  ou au dessus du 100% de la population (a posteriori en tenant compte de toutes les mesures ?)</t>
   </si>
   <si>
@@ -120,6 +117,9 @@
   </si>
   <si>
     <t>Warning dans le rapport</t>
+  </si>
+  <si>
+    <t>Si des requêtes sont présentes les ignorer ? Ok/ faire une reuqête custom pour tuberXpert</t>
   </si>
 </sst>
 </file>
@@ -504,7 +504,7 @@
   <dimension ref="B3:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -559,13 +559,13 @@
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="45" x14ac:dyDescent="0.25">
@@ -573,7 +573,7 @@
         <v>12</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>13</v>
@@ -595,7 +595,7 @@
         <v>14</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>17</v>
@@ -606,10 +606,10 @@
         <v>18</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Writing checks in official documentation
</commit_message>
<xml_diff>
--- a/publi/checks.xlsx
+++ b/publi/checks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\melvy\Desktop\Dev\2022-herzig\publi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0E7150E-C0B6-4B42-95EA-D2CE0FCF9736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{109F2767-8904-4A0F-B8E7-B5373822B441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7459B878-47C4-4386-AB9E-890DDB192382}"/>
+    <workbookView xWindow="-27330" yWindow="915" windowWidth="26505" windowHeight="14100" xr2:uid="{7459B878-47C4-4386-AB9E-890DDB192382}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>drug/drugId</t>
   </si>
@@ -100,9 +100,6 @@
     <t xml:space="preserve">Request </t>
   </si>
   <si>
-    <t>Vérifier que la valeur d'un sample ne soit pas en dessous du 0 pourcent  ou au dessus du 100% de la population (a posteriori en tenant compte de toutes les mesures ?)</t>
-  </si>
-  <si>
     <t>Si deux targets ont le même activeMoietyId et le même targetType ou
 si l'activeMoityId n'appartient pas au médicament</t>
   </si>
@@ -120,6 +117,14 @@
   </si>
   <si>
     <t>Si des requêtes sont présentes les ignorer ? Ok/ faire une reuqête custom pour tuberXpert</t>
+  </si>
+  <si>
+    <t>Vérifier que la valeur d'un sample ne soit pas en dessous du 0 pourcent  ou au dessus du 100% de la population</t>
+  </si>
+  <si>
+    <t>peut être utile pour spécifier le type de sortie (html, pdf …) 
+le type de computation (locale, distante) , le fait d'autoriser ou refuser
+ les doses de charge et le temps de repo</t>
   </si>
 </sst>
 </file>
@@ -143,12 +148,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -178,7 +189,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -186,6 +197,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -504,7 +518,7 @@
   <dimension ref="B3:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C17" sqref="C15:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -525,7 +539,7 @@
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -536,7 +550,7 @@
       </c>
     </row>
     <row r="5" spans="2:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -547,7 +561,7 @@
       </c>
     </row>
     <row r="6" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -559,28 +573,28 @@
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
+    </row>
+    <row r="8" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -591,11 +605,11 @@
       </c>
     </row>
     <row r="10" spans="2:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>17</v>
@@ -606,15 +620,17 @@
         <v>18</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="60" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
+      <c r="C12" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="D12" s="3"/>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Specification and other official documents
</commit_message>
<xml_diff>
--- a/publi/checks.xlsx
+++ b/publi/checks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\melvy\Desktop\Dev\2022-herzig\publi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{109F2767-8904-4A0F-B8E7-B5373822B441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D472C92-6C0C-4A60-81F5-ED0D821FE397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27330" yWindow="915" windowWidth="26505" windowHeight="14100" xr2:uid="{7459B878-47C4-4386-AB9E-890DDB192382}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7459B878-47C4-4386-AB9E-890DDB192382}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -113,9 +113,6 @@
     <t>Vérifier que la valeur d'un sample ne soit pas en dehors des limites</t>
   </si>
   <si>
-    <t>Warning dans le rapport</t>
-  </si>
-  <si>
     <t>Si des requêtes sont présentes les ignorer ? Ok/ faire une reuqête custom pour tuberXpert</t>
   </si>
   <si>
@@ -125,6 +122,9 @@
     <t>peut être utile pour spécifier le type de sortie (html, pdf …) 
 le type de computation (locale, distante) , le fait d'autoriser ou refuser
  les doses de charge et le temps de repo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Warning dans le rapport Fort &lt; 5 || &gt; 94  et failble &lt; 10 || &gt; 90 </t>
   </si>
 </sst>
 </file>
@@ -518,7 +518,7 @@
   <dimension ref="B3:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C15:C17"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,7 +579,7 @@
         <v>22</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="30" x14ac:dyDescent="0.25">
@@ -587,7 +587,7 @@
         <v>12</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>13</v>
@@ -620,7 +620,7 @@
         <v>18</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>20</v>
@@ -629,7 +629,7 @@
     <row r="12" spans="2:4" ht="60" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
       <c r="C12" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D12" s="3"/>
     </row>

</xml_diff>

<commit_message>
Questions for 08 04 meeting
</commit_message>
<xml_diff>
--- a/publi/checks.xlsx
+++ b/publi/checks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\melvy\Desktop\Dev\2022-herzig\publi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D472C92-6C0C-4A60-81F5-ED0D821FE397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEF4F449-EA96-4D8E-8F57-FDA1515AC425}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7459B878-47C4-4386-AB9E-890DDB192382}"/>
+    <workbookView xWindow="-28065" yWindow="600" windowWidth="26505" windowHeight="14100" xr2:uid="{7459B878-47C4-4386-AB9E-890DDB192382}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -124,7 +124,7 @@
  les doses de charge et le temps de repo</t>
   </si>
   <si>
-    <t xml:space="preserve">Warning dans le rapport Fort &lt; 5 || &gt; 94  et failble &lt; 10 || &gt; 90 </t>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>

</xml_diff>